<commit_message>
Set up second big run (partial)
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2201510-CC71-4937-85FE-329D9876F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9D843D-F074-4906-90BB-56A91D80D5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="5115" windowWidth="28800" windowHeight="15345" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Parameter</t>
   </si>
@@ -235,27 +235,15 @@
     <t>value2</t>
   </si>
   <si>
-    <t>yolov8 s/m</t>
-  </si>
-  <si>
     <t>Use extra</t>
   </si>
   <si>
     <t>15 to 45</t>
   </si>
   <si>
-    <t>Either - increase epochs</t>
-  </si>
-  <si>
-    <t>X - test</t>
-  </si>
-  <si>
     <t>0 or  0.4</t>
   </si>
   <si>
-    <t>10^-3.5 to 10^-2.5</t>
-  </si>
-  <si>
     <t>Turning off is bad in intermediate_weights_many</t>
   </si>
   <si>
@@ -268,23 +256,104 @@
     <t>0 to 4</t>
   </si>
   <si>
-    <t>0 to 0.1</t>
-  </si>
-  <si>
-    <t>1 to 7.5</t>
-  </si>
-  <si>
-    <t>0 to 15</t>
-  </si>
-  <si>
     <t>z_range</t>
+  </si>
+  <si>
+    <t>4 (1 for local)</t>
+  </si>
+  <si>
+    <t>0 to 2</t>
+  </si>
+  <si>
+    <t>20 to 70</t>
+  </si>
+  <si>
+    <t>4 to 7.5</t>
+  </si>
+  <si>
+    <t>yolov8 s/m, yolov10 s/m</t>
+  </si>
+  <si>
+    <t>20 to 25</t>
+  </si>
+  <si>
+    <t>0 to 0.1 (50% 0)</t>
+  </si>
+  <si>
+    <t>0.6 to 0.65</t>
+  </si>
+  <si>
+    <t>480 to 640</t>
+  </si>
+  <si>
+    <t>10^-3.2 to 10^-2.8</t>
+  </si>
+  <si>
+    <t>14 to 30</t>
+  </si>
+  <si>
+    <t>0.0001 to 0.0006</t>
+  </si>
+  <si>
+    <t>0 or 0.1</t>
+  </si>
+  <si>
+    <t>0.25 to 0.6</t>
+  </si>
+  <si>
+    <t>individual extra data</t>
+  </si>
+  <si>
+    <t>0 to 0.2</t>
+  </si>
+  <si>
+    <t>2000 to 4000</t>
+  </si>
+  <si>
+    <t>edge padding</t>
+  </si>
+  <si>
+    <t>Scale 1 to 1.5</t>
+  </si>
+  <si>
+    <t>10 to 20</t>
+  </si>
+  <si>
+    <t>0 to 60</t>
+  </si>
+  <si>
+    <t>2.5 to 3.5</t>
+  </si>
+  <si>
+    <t>2 to 4</t>
+  </si>
+  <si>
+    <t>0 to 0.015</t>
+  </si>
+  <si>
+    <t>0 to 0.4</t>
+  </si>
+  <si>
+    <t>0 to 0.7</t>
+  </si>
+  <si>
+    <t>0 or 0.5</t>
+  </si>
+  <si>
+    <t>3 to 6</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3 modes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +371,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,11 +405,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,8 +430,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:F51" totalsRowShown="0">
-  <autoFilter ref="A1:F51" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:F53" totalsRowShown="0">
+  <autoFilter ref="A1:F53" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F47">
     <sortCondition ref="B1:B47"/>
   </sortState>
@@ -664,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A27ABA-385A-41E0-AC82-8511CBF6AE11}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,7 +755,7 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="41" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" customWidth="1"/>
     <col min="6" max="6" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -709,8 +789,8 @@
       <c r="C2" t="s">
         <v>61</v>
       </c>
-      <c r="D2">
-        <v>4</v>
+      <c r="D2" t="s">
+        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -730,7 +810,7 @@
         <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -764,7 +844,7 @@
         <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
@@ -781,7 +861,7 @@
         <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>58</v>
@@ -798,7 +878,7 @@
         <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
         <v>59</v>
@@ -819,7 +899,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B9">
@@ -833,7 +913,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B10">
@@ -842,12 +922,12 @@
       <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>71</v>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -861,7 +941,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B12">
@@ -875,7 +955,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B13">
@@ -884,12 +964,12 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13">
-        <v>20</v>
+      <c r="D13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B14">
@@ -899,11 +979,11 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B15">
@@ -913,11 +993,11 @@
         <v>7.5</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B16">
@@ -926,12 +1006,12 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B17">
@@ -944,8 +1024,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B18">
@@ -958,8 +1038,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B19">
@@ -968,12 +1048,12 @@
       <c r="C19">
         <v>0.6</v>
       </c>
-      <c r="D19">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B20">
@@ -982,12 +1062,12 @@
       <c r="C20">
         <v>640</v>
       </c>
-      <c r="D20">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B21">
@@ -997,11 +1077,11 @@
         <v>1E-3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B22">
@@ -1010,12 +1090,12 @@
       <c r="C22">
         <v>18</v>
       </c>
-      <c r="D22">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B23">
@@ -1028,8 +1108,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B24">
@@ -1038,12 +1118,12 @@
       <c r="C24">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="D24">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B25">
@@ -1052,12 +1132,12 @@
       <c r="C25">
         <v>0.1</v>
       </c>
-      <c r="D25">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B26">
@@ -1066,12 +1146,16 @@
       <c r="C26">
         <v>0.5</v>
       </c>
-      <c r="D26">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J26">
+        <f>32*20</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B27">
@@ -1083,9 +1167,13 @@
       <c r="D27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="J27">
+        <f>32*15</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B28">
@@ -1095,11 +1183,11 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B29">
@@ -1108,15 +1196,15 @@
       <c r="C29">
         <v>0.2</v>
       </c>
-      <c r="D29">
-        <v>0.2</v>
+      <c r="D29" t="s">
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B30">
@@ -1126,11 +1214,11 @@
         <v>0.4</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1143,8 +1231,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1158,7 +1246,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -1167,12 +1255,12 @@
       <c r="C33">
         <v>10</v>
       </c>
-      <c r="D33">
-        <v>10</v>
+      <c r="D33" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B34">
@@ -1181,12 +1269,12 @@
       <c r="C34">
         <v>3000</v>
       </c>
-      <c r="D34">
-        <v>3000</v>
+      <c r="D34" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B35">
@@ -1195,12 +1283,12 @@
       <c r="C35">
         <v>3000</v>
       </c>
-      <c r="D35">
-        <v>3000</v>
+      <c r="D35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B36">
@@ -1209,12 +1297,12 @@
       <c r="C36">
         <v>60</v>
       </c>
-      <c r="D36">
-        <v>60</v>
+      <c r="D36" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B37">
@@ -1223,12 +1311,12 @@
       <c r="C37">
         <v>3</v>
       </c>
-      <c r="D37">
-        <v>3</v>
+      <c r="D37" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B38">
@@ -1237,12 +1325,12 @@
       <c r="C38">
         <v>3</v>
       </c>
-      <c r="D38">
-        <v>3</v>
+      <c r="D38" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B39">
@@ -1251,12 +1339,12 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>73</v>
+      <c r="D39" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B40">
@@ -1270,7 +1358,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B41">
@@ -1279,12 +1367,12 @@
       <c r="C41">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D41">
-        <v>1.4999999999999999E-2</v>
+      <c r="D41" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B42">
@@ -1293,12 +1381,12 @@
       <c r="C42">
         <v>0.7</v>
       </c>
-      <c r="D42">
-        <v>0.7</v>
+      <c r="D42" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B43">
@@ -1307,12 +1395,12 @@
       <c r="C43">
         <v>0.4</v>
       </c>
-      <c r="D43">
-        <v>0.4</v>
+      <c r="D43" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B44">
@@ -1321,12 +1409,12 @@
       <c r="C44">
         <v>0.5</v>
       </c>
-      <c r="D44">
-        <v>0.5</v>
+      <c r="D44" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B45">
@@ -1335,12 +1423,12 @@
       <c r="C45">
         <v>0.5</v>
       </c>
-      <c r="D45">
-        <v>0.5</v>
+      <c r="D45" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B46">
@@ -1354,7 +1442,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B47">
@@ -1368,7 +1456,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B48">
@@ -1377,12 +1465,12 @@
       <c r="C48">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
-        <v>72</v>
+      <c r="D48">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B49">
@@ -1392,12 +1480,12 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>77</v>
+      <c r="A50" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="B50">
         <v>2</v>
@@ -1406,12 +1494,12 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>83</v>
+      <c r="A51" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1419,8 +1507,30 @@
       <c r="C51">
         <v>-1</v>
       </c>
-      <c r="D51">
-        <v>-1</v>
+      <c r="D51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak a bit more
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9D843D-F074-4906-90BB-56A91D80D5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB3CFD2-E31E-4FCB-8132-1529FE5698BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="108">
   <si>
     <t>Parameter</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>3 modes</t>
+  </si>
+  <si>
+    <t>0.2, or 0 (and 0.01 absolute)</t>
   </si>
 </sst>
 </file>
@@ -410,8 +413,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,7 +750,7 @@
   <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +902,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9">
@@ -913,7 +916,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10">
@@ -922,12 +925,12 @@
       <c r="C10">
         <v>30</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
       <c r="B11">
@@ -941,7 +944,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
       <c r="B12">
@@ -955,7 +958,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13">
@@ -969,7 +972,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" t="s">
         <v>47</v>
       </c>
       <c r="B14">
@@ -983,7 +986,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15">
@@ -997,7 +1000,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B16">
@@ -1011,7 +1014,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
         <v>52</v>
       </c>
       <c r="B17">
@@ -1025,7 +1028,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>45</v>
       </c>
       <c r="B18">
@@ -1039,7 +1042,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="B19">
@@ -1053,7 +1056,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20">
@@ -1067,7 +1070,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
       <c r="B21">
@@ -1081,7 +1084,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>12</v>
       </c>
       <c r="B22">
@@ -1095,7 +1098,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23">
@@ -1109,7 +1112,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
       <c r="B24">
@@ -1123,7 +1126,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>19</v>
       </c>
       <c r="B25">
@@ -1137,7 +1140,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>20</v>
       </c>
       <c r="B26">
@@ -1155,7 +1158,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B27">
@@ -1173,7 +1176,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
       <c r="B28">
@@ -1187,7 +1190,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
       <c r="B29">
@@ -1204,7 +1207,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
       <c r="B30">
@@ -1218,7 +1221,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
@@ -1241,12 +1244,12 @@
       <c r="C32">
         <v>0.2</v>
       </c>
-      <c r="D32">
-        <v>0.2</v>
+      <c r="D32" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33">
@@ -1260,7 +1263,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34">
@@ -1274,7 +1277,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" t="s">
         <v>40</v>
       </c>
       <c r="B35">
@@ -1288,7 +1291,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" t="s">
         <v>41</v>
       </c>
       <c r="B36">
@@ -1302,7 +1305,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
       <c r="B37">
@@ -1316,7 +1319,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38">
@@ -1330,7 +1333,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" t="s">
         <v>11</v>
       </c>
       <c r="B39">
@@ -1339,12 +1342,12 @@
       <c r="C39">
         <v>1</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" t="s">
         <v>14</v>
       </c>
       <c r="B40">
@@ -1358,7 +1361,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" t="s">
         <v>16</v>
       </c>
       <c r="B41">
@@ -1372,7 +1375,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+      <c r="A42" t="s">
         <v>17</v>
       </c>
       <c r="B42">
@@ -1386,7 +1389,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" t="s">
         <v>18</v>
       </c>
       <c r="B43">
@@ -1400,7 +1403,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" t="s">
         <v>21</v>
       </c>
       <c r="B44">
@@ -1414,7 +1417,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="A45" t="s">
         <v>22</v>
       </c>
       <c r="B45">
@@ -1428,7 +1431,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" t="s">
         <v>24</v>
       </c>
       <c r="B46">
@@ -1442,7 +1445,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
       <c r="B47">
@@ -1456,7 +1459,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="A48" t="s">
         <v>53</v>
       </c>
       <c r="B48">
@@ -1470,7 +1473,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" t="s">
         <v>66</v>
       </c>
       <c r="B49">
@@ -1484,7 +1487,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" t="s">
         <v>73</v>
       </c>
       <c r="B50">
@@ -1498,7 +1501,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" t="s">
         <v>76</v>
       </c>
       <c r="B51">
@@ -1523,7 +1526,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>94</v>
       </c>
       <c r="C53">

</xml_diff>

<commit_message>
Add small tester for degrees and blur_z
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB3CFD2-E31E-4FCB-8132-1529FE5698BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456D4D8-9CC2-4CCF-9506-C6DBCEE5C287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
   <si>
     <t>Parameter</t>
   </si>
@@ -350,22 +350,17 @@
   </si>
   <si>
     <t>0.2, or 0 (and 0.01 absolute)</t>
+  </si>
+  <si>
+    <t>DETR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -408,12 +403,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -433,8 +427,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:F53" totalsRowShown="0">
-  <autoFilter ref="A1:F53" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0">
+  <autoFilter ref="A1:F54" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F47">
     <sortCondition ref="B1:B47"/>
   </sortState>
@@ -747,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A27ABA-385A-41E0-AC82-8511CBF6AE11}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,10 +837,10 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E5" t="s">
@@ -1000,7 +994,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B16">
@@ -1037,7 +1031,7 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1076,10 +1070,10 @@
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>1E-3</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1158,7 +1152,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B27">
@@ -1235,7 +1229,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1515,7 +1509,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="A52" t="s">
         <v>91</v>
       </c>
       <c r="C52" t="s">
@@ -1526,7 +1520,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C53">
@@ -1536,8 +1530,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Tweak runner, production candidate for run 2
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9456D4D8-9CC2-4CCF-9506-C6DBCEE5C287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA190E23-454E-41A2-9366-D7C6F3167508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="111">
   <si>
     <t>Parameter</t>
   </si>
@@ -340,9 +340,6 @@
     <t>0 or 0.5</t>
   </si>
   <si>
-    <t>3 to 6</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>DETR</t>
+  </si>
+  <si>
+    <t>0 or 10</t>
+  </si>
+  <si>
+    <t>0 or 15</t>
+  </si>
+  <si>
+    <t>0 or (3 to 6)</t>
   </si>
 </sst>
 </file>
@@ -744,7 +750,7 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,7 +1000,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B16">
@@ -1003,8 +1009,8 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="D16">
-        <v>0</v>
+      <c r="D16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1152,7 +1158,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B27">
@@ -1161,8 +1167,8 @@
       <c r="C27">
         <v>0</v>
       </c>
-      <c r="D27">
-        <v>0</v>
+      <c r="D27" t="s">
+        <v>108</v>
       </c>
       <c r="J27">
         <f>32*15</f>
@@ -1180,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1229,7 +1235,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
@@ -1239,7 +1245,7 @@
         <v>0.2</v>
       </c>
       <c r="D32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1511,7 @@
         <v>-1</v>
       </c>
       <c r="D51" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1513,10 +1519,10 @@
         <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1532,7 +1538,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweak runner for next run / labeling
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D69F64-1A07-4D91-A277-9A8A9574929C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93F3285-D027-4CB4-9098-B9FF09D23565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="178">
   <si>
     <t>Parameter</t>
   </si>
@@ -410,6 +410,156 @@
   </si>
   <si>
     <t>20 to 50</t>
+  </si>
+  <si>
+    <t>Observations2</t>
+  </si>
+  <si>
+    <t>Helps, p=0.0001, higher than 0.2 needed?</t>
+  </si>
+  <si>
+    <t>value4</t>
+  </si>
+  <si>
+    <t>Helps, p=0.000 (?)</t>
+  </si>
+  <si>
+    <t>-1 is bad</t>
+  </si>
+  <si>
+    <t>No impact in CV but very bad on Kaggle</t>
+  </si>
+  <si>
+    <t>Absolute is bad on Kaggle</t>
+  </si>
+  <si>
+    <t>Adjusting upwards helps on Kaggle</t>
+  </si>
+  <si>
+    <t>Not considered</t>
+  </si>
+  <si>
+    <t>1 (ensemble later)</t>
+  </si>
+  <si>
+    <t>Lower a bit better? No clear relationship</t>
+  </si>
+  <si>
+    <t>20 to 40</t>
+  </si>
+  <si>
+    <t>0 is bad, 2 a bit better in CV</t>
+  </si>
+  <si>
+    <t>v8m only</t>
+  </si>
+  <si>
+    <t>8 is best, v8m beats v8s on kaggle</t>
+  </si>
+  <si>
+    <t>0.45 (optimize post)</t>
+  </si>
+  <si>
+    <t>Higher slightly better on Kaggle?</t>
+  </si>
+  <si>
+    <t>30 to 45</t>
+  </si>
+  <si>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>Smaller slightly better on Kaggle?</t>
+  </si>
+  <si>
+    <t>18 to 20</t>
+  </si>
+  <si>
+    <t>0 to 0.1</t>
+  </si>
+  <si>
+    <t>Lower seems better</t>
+  </si>
+  <si>
+    <t>1 to 5</t>
+  </si>
+  <si>
+    <t>1 to 2</t>
+  </si>
+  <si>
+    <t>Smaller slightly better?</t>
+  </si>
+  <si>
+    <t>No relationship</t>
+  </si>
+  <si>
+    <t>Bigger slightly better?</t>
+  </si>
+  <si>
+    <t>576 to 640</t>
+  </si>
+  <si>
+    <t>0.3 to 0.6</t>
+  </si>
+  <si>
+    <t>0 is bad in CV but good on Kaggle, small value seems helpful</t>
+  </si>
+  <si>
+    <t>Mosaic seems to prevent some bad models</t>
+  </si>
+  <si>
+    <t>0.2 to 1</t>
+  </si>
+  <si>
+    <t>0.1 to 0.2 (0 absolute)</t>
+  </si>
+  <si>
+    <t>1500 to 3000</t>
+  </si>
+  <si>
+    <t>Higher a bit better?</t>
+  </si>
+  <si>
+    <t>Scale 1.5 to 2.5</t>
+  </si>
+  <si>
+    <t>Lower a tiny bit better?</t>
+  </si>
+  <si>
+    <t>Perhaps a tiny bit better in latest experiment…</t>
+  </si>
+  <si>
+    <t>Helps, p=0.002, not as much on Kaggle</t>
+  </si>
+  <si>
+    <t>0 is bad, a bit lower may be best on Kaggle</t>
+  </si>
+  <si>
+    <t>3 to 6</t>
+  </si>
+  <si>
+    <t>Lower better?</t>
+  </si>
+  <si>
+    <t>0.907 to 0.937</t>
+  </si>
+  <si>
+    <t>0.9 to 1.3</t>
+  </si>
+  <si>
+    <t>1 to 1.4</t>
+  </si>
+  <si>
+    <t>rgb_offset</t>
+  </si>
+  <si>
+    <t>pad_with_noise</t>
+  </si>
+  <si>
+    <t>ignore_suspect_positives</t>
+  </si>
+  <si>
+    <t>include_multi_motor</t>
   </si>
 </sst>
 </file>
@@ -432,7 +582,6 @@
     </font>
     <font>
       <b/>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -460,11 +609,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,18 +633,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:G60" totalsRowShown="0">
-  <autoFilter ref="A1:G60" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:I64" totalsRowShown="0">
+  <autoFilter ref="A1:I64" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
     <sortCondition ref="B1:B47"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{245421F4-54AE-4BC8-AE08-C40E10577FB1}" name="Parameter"/>
     <tableColumn id="2" xr3:uid="{12D688A8-92E6-4707-94A6-424E10AEDD68}" name="Tier"/>
     <tableColumn id="6" xr3:uid="{34671572-2E72-44A5-A805-B3D52876428F}" name="value1"/>
     <tableColumn id="8" xr3:uid="{5F31E01E-98B1-4F2C-84AA-EB9826BFDB08}" name="value2"/>
     <tableColumn id="5" xr3:uid="{8328DEA5-1ECC-42EC-95C8-FCAFE61AC7DB}" name="value3"/>
+    <tableColumn id="9" xr3:uid="{61282190-3514-4D5A-9262-8F241FFE328A}" name="value4"/>
     <tableColumn id="3" xr3:uid="{3FACB684-5B57-4900-BF32-BDEDEE73ABA9}" name="Observations1"/>
+    <tableColumn id="7" xr3:uid="{7BE35C65-6771-483E-8F03-97F85FDBD339}" name="Observations2"/>
     <tableColumn id="4" xr3:uid="{2055747C-492F-4C34-84F5-9F642C958466}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -798,10 +950,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A27ABA-385A-41E0-AC82-8511CBF6AE11}">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,12 +962,12 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" customWidth="1"/>
-    <col min="7" max="7" width="51.28515625" customWidth="1"/>
+    <col min="5" max="6" width="52.7109375" customWidth="1"/>
+    <col min="7" max="8" width="41.85546875" customWidth="1"/>
+    <col min="9" max="9" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -831,13 +984,19 @@
         <v>116</v>
       </c>
       <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -853,14 +1012,20 @@
       <c r="E2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -877,10 +1042,16 @@
         <v>127</v>
       </c>
       <c r="F3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -896,11 +1067,17 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -916,12 +1093,18 @@
       <c r="E5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="H5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -937,10 +1120,16 @@
         <v>117</v>
       </c>
       <c r="F6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -957,10 +1146,16 @@
         <v>69</v>
       </c>
       <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -976,8 +1171,14 @@
       <c r="E8">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -993,8 +1194,14 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1010,8 +1217,14 @@
       <c r="E10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1027,8 +1240,14 @@
       <c r="E11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1044,8 +1263,14 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1061,8 +1286,14 @@
       <c r="E13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1078,8 +1309,14 @@
       <c r="E14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1095,8 +1332,14 @@
       <c r="E15" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1112,8 +1355,14 @@
       <c r="E16" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1129,8 +1378,14 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1146,8 +1401,14 @@
       <c r="E18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1163,8 +1424,14 @@
       <c r="E19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="H19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1180,8 +1447,14 @@
       <c r="E20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1197,8 +1470,14 @@
       <c r="E21" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1214,8 +1493,14 @@
       <c r="E22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1231,8 +1516,14 @@
       <c r="E23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="H23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1248,8 +1539,14 @@
       <c r="E24" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1265,8 +1562,14 @@
       <c r="E25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1282,8 +1585,14 @@
       <c r="E26" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1299,8 +1608,14 @@
       <c r="E27" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1316,8 +1631,14 @@
       <c r="E28" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1334,10 +1655,16 @@
         <v>92</v>
       </c>
       <c r="F29" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1353,8 +1680,14 @@
       <c r="E30" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1370,8 +1703,14 @@
       <c r="E31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1387,8 +1726,14 @@
       <c r="E32" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1404,8 +1749,14 @@
       <c r="E33" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1421,8 +1772,14 @@
       <c r="E34" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1438,8 +1795,14 @@
       <c r="E35" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1455,8 +1818,14 @@
       <c r="E36" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="H36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1472,8 +1841,14 @@
       <c r="E37" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1489,9 +1864,15 @@
       <c r="E38" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+      <c r="H38" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B39">
@@ -1506,8 +1887,14 @@
       <c r="E39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1523,8 +1910,14 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="H40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1540,8 +1933,14 @@
       <c r="E41" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1557,8 +1956,14 @@
       <c r="E42" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1574,8 +1979,14 @@
       <c r="E43" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -1591,8 +2002,14 @@
       <c r="E44" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>0.5</v>
+      </c>
+      <c r="H44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1608,8 +2025,14 @@
       <c r="E45" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>0.5</v>
+      </c>
+      <c r="H45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -1625,8 +2048,14 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="H46" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -1642,8 +2071,14 @@
       <c r="E47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1659,8 +2094,14 @@
       <c r="E48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -1676,8 +2117,14 @@
       <c r="E49" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -1693,8 +2140,14 @@
       <c r="E50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -1710,8 +2163,14 @@
       <c r="E51" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -1724,8 +2183,14 @@
       <c r="E52" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -1738,8 +2203,14 @@
       <c r="E53" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>103</v>
+      </c>
+      <c r="H53" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -1752,8 +2223,14 @@
       <c r="E54" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>171</v>
+      </c>
+      <c r="H54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -1766,8 +2243,14 @@
       <c r="E55" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>3</v>
+      </c>
+      <c r="H55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -1780,9 +2263,15 @@
       <c r="E56" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="F56">
+        <v>0.01</v>
+      </c>
+      <c r="H56" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C57">
@@ -1794,9 +2283,15 @@
       <c r="E57" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="F57" t="s">
+        <v>124</v>
+      </c>
+      <c r="H57" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C58">
@@ -1808,9 +2303,15 @@
       <c r="E58" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="F58" t="s">
+        <v>172</v>
+      </c>
+      <c r="H58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C59">
@@ -1822,9 +2323,15 @@
       <c r="E59" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="F59" t="s">
+        <v>173</v>
+      </c>
+      <c r="H59" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>115</v>
       </c>
       <c r="C60">
@@ -1835,6 +2342,32 @@
       </c>
       <c r="E60" t="s">
         <v>126</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="H60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove old files / tweak runner / add min img size
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55707401-B051-42F1-86C9-009BDD6DC611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEDB86C-99FE-462A-AF32-D47B117D3A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="181">
   <si>
     <t>Parameter</t>
   </si>
@@ -563,6 +563,12 @@
   </si>
   <si>
     <t>min size</t>
+  </si>
+  <si>
+    <t>[0.,1.,15.,30.,45.,60.,100.]</t>
+  </si>
+  <si>
+    <t>0 to 0.5</t>
   </si>
 </sst>
 </file>
@@ -612,11 +618,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,7 +963,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,28 +2360,43 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="4" t="s">
         <v>174</v>
       </c>
+      <c r="F61" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="4" t="s">
         <v>175</v>
       </c>
+      <c r="F62" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="4" t="s">
         <v>176</v>
       </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="4" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>178</v>
+      </c>
+      <c r="F65" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update runner for vals5
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEDB86C-99FE-462A-AF32-D47B117D3A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE87AB50-5C70-49FC-8C3E-BFDFF07FEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="196">
   <si>
     <t>Parameter</t>
   </si>
@@ -569,6 +569,51 @@
   </si>
   <si>
     <t>0 to 0.5</t>
+  </si>
+  <si>
+    <t>value5</t>
+  </si>
+  <si>
+    <t>Some poor ones at 20 to 25</t>
+  </si>
+  <si>
+    <t>25 to 40</t>
+  </si>
+  <si>
+    <t>v8m or v8l</t>
+  </si>
+  <si>
+    <t>20 to 22</t>
+  </si>
+  <si>
+    <t>Increase a bit for speed</t>
+  </si>
+  <si>
+    <t>2000 to 3500</t>
+  </si>
+  <si>
+    <t>Scale 2 to 2.5</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Higher is better</t>
+  </si>
+  <si>
+    <t>3 to 3.7</t>
+  </si>
+  <si>
+    <t>2.5 to 4.5</t>
+  </si>
+  <si>
+    <t>0.922 to 0.942</t>
+  </si>
+  <si>
+    <t>Observations4</t>
+  </si>
+  <si>
+    <t>1 to 4</t>
   </si>
 </sst>
 </file>
@@ -618,12 +663,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,20 +686,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:I65" totalsRowShown="0">
-  <autoFilter ref="A1:I65" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}" name="Table1" displayName="Table1" ref="A1:K65" totalsRowShown="0">
+  <autoFilter ref="A1:K65" xr:uid="{4BF53FAF-C3F4-4CAF-8CD1-B81AF65BECC4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K47">
     <sortCondition ref="B1:B47"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{245421F4-54AE-4BC8-AE08-C40E10577FB1}" name="Parameter"/>
     <tableColumn id="2" xr3:uid="{12D688A8-92E6-4707-94A6-424E10AEDD68}" name="Tier"/>
     <tableColumn id="6" xr3:uid="{34671572-2E72-44A5-A805-B3D52876428F}" name="value1"/>
     <tableColumn id="8" xr3:uid="{5F31E01E-98B1-4F2C-84AA-EB9826BFDB08}" name="value2"/>
     <tableColumn id="5" xr3:uid="{8328DEA5-1ECC-42EC-95C8-FCAFE61AC7DB}" name="value3"/>
     <tableColumn id="9" xr3:uid="{61282190-3514-4D5A-9262-8F241FFE328A}" name="value4"/>
+    <tableColumn id="11" xr3:uid="{3AF65E23-F4A6-4494-A69C-8299F4E840B7}" name="value5"/>
     <tableColumn id="3" xr3:uid="{3FACB684-5B57-4900-BF32-BDEDEE73ABA9}" name="Observations1"/>
     <tableColumn id="7" xr3:uid="{7BE35C65-6771-483E-8F03-97F85FDBD339}" name="Observations2"/>
+    <tableColumn id="10" xr3:uid="{6355B6F2-4AB7-4995-9759-B38F60A81164}" name="Observations4"/>
     <tableColumn id="4" xr3:uid="{2055747C-492F-4C34-84F5-9F642C958466}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -959,11 +1005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A27ABA-385A-41E0-AC82-8511CBF6AE11}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,12 +1017,13 @@
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="6" width="52.7109375" customWidth="1"/>
-    <col min="7" max="8" width="41.85546875" customWidth="1"/>
-    <col min="9" max="9" width="51.28515625" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" customWidth="1"/>
+    <col min="6" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="10" width="41.85546875" customWidth="1"/>
+    <col min="11" max="11" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -996,16 +1043,22 @@
         <v>130</v>
       </c>
       <c r="G1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" t="s">
         <v>67</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>128</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1024,17 +1077,20 @@
       <c r="F2" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
         <v>54</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>136</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1054,13 +1110,19 @@
         <v>139</v>
       </c>
       <c r="G3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H3" t="s">
         <v>55</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1079,14 +1141,17 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>56</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1105,14 +1170,17 @@
       <c r="F5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
         <v>57</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1132,13 +1200,16 @@
         <v>141</v>
       </c>
       <c r="G6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1158,13 +1229,16 @@
         <v>69</v>
       </c>
       <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" t="s">
         <v>59</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1183,11 +1257,14 @@
       <c r="F8" t="s">
         <v>143</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1206,11 +1283,14 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1229,11 +1309,14 @@
       <c r="F10" t="s">
         <v>145</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1252,11 +1335,14 @@
       <c r="F11" t="s">
         <v>146</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1275,11 +1361,14 @@
       <c r="F12">
         <v>1</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1298,11 +1387,17 @@
       <c r="F13" t="s">
         <v>148</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
+        <v>185</v>
+      </c>
+      <c r="I13" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -1321,11 +1416,14 @@
       <c r="F14" t="s">
         <v>149</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1344,11 +1442,14 @@
       <c r="F15" t="s">
         <v>151</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
+        <v>195</v>
+      </c>
+      <c r="I15" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1367,11 +1468,14 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1390,11 +1494,14 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1413,11 +1520,14 @@
       <c r="F18" s="1">
         <v>1</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1436,11 +1546,14 @@
       <c r="F19" t="s">
         <v>84</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+      <c r="I19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1459,11 +1572,14 @@
       <c r="F20" t="s">
         <v>156</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1482,11 +1598,14 @@
       <c r="F21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I21" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1505,11 +1624,14 @@
       <c r="F22" t="s">
         <v>87</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1528,11 +1650,14 @@
       <c r="F23">
         <v>4</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1551,11 +1676,14 @@
       <c r="F24" t="s">
         <v>119</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
+        <v>119</v>
+      </c>
+      <c r="I24" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1574,11 +1702,14 @@
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="H25" t="s">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1597,11 +1728,14 @@
       <c r="F26" t="s">
         <v>157</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1620,11 +1754,14 @@
       <c r="F27">
         <v>10</v>
       </c>
-      <c r="H27" t="s">
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1643,11 +1780,14 @@
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="H28" t="s">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1667,13 +1807,16 @@
         <v>160</v>
       </c>
       <c r="G29" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" t="s">
         <v>72</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1690,13 +1833,16 @@
         <v>71</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
-      </c>
-      <c r="H30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30" t="s">
+        <v>100</v>
+      </c>
+      <c r="I30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1715,11 +1861,14 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="H31" t="s">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1738,11 +1887,14 @@
       <c r="F32" t="s">
         <v>161</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G32" t="s">
+        <v>161</v>
+      </c>
+      <c r="I32" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1761,11 +1913,14 @@
       <c r="F33">
         <v>10</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="I33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1784,11 +1939,14 @@
       <c r="F34" t="s">
         <v>162</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1807,11 +1965,14 @@
       <c r="F35" t="s">
         <v>164</v>
       </c>
-      <c r="H35" t="s">
+      <c r="G35" t="s">
+        <v>188</v>
+      </c>
+      <c r="I35" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1830,11 +1991,14 @@
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="H36" t="s">
+      <c r="G36" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I36" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1853,11 +2017,17 @@
       <c r="F37" t="s">
         <v>97</v>
       </c>
-      <c r="H37" t="s">
+      <c r="G37" t="s">
+        <v>191</v>
+      </c>
+      <c r="I37" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1876,11 +2046,14 @@
       <c r="F38" t="s">
         <v>98</v>
       </c>
-      <c r="H38" t="s">
+      <c r="G38" t="s">
+        <v>192</v>
+      </c>
+      <c r="I38" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1899,11 +2072,14 @@
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -1922,11 +2098,14 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -1945,11 +2124,14 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="H41" t="s">
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>17</v>
       </c>
@@ -1968,11 +2150,14 @@
       <c r="F42">
         <v>0</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1991,11 +2176,14 @@
       <c r="F43">
         <v>0</v>
       </c>
-      <c r="H43" t="s">
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>21</v>
       </c>
@@ -2014,11 +2202,14 @@
       <c r="F44">
         <v>0.5</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G44">
+        <v>0.5</v>
+      </c>
+      <c r="I44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -2037,11 +2228,14 @@
       <c r="F45">
         <v>0.5</v>
       </c>
-      <c r="H45" t="s">
+      <c r="G45">
+        <v>0.5</v>
+      </c>
+      <c r="I45" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -2060,11 +2254,14 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>28</v>
       </c>
@@ -2083,11 +2280,14 @@
       <c r="F47">
         <v>0</v>
       </c>
-      <c r="H47" t="s">
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -2106,11 +2306,14 @@
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="H48" t="s">
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="I48" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>66</v>
       </c>
@@ -2129,11 +2332,14 @@
       <c r="F49" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H49" t="s">
+      <c r="G49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I49" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>73</v>
       </c>
@@ -2152,11 +2358,14 @@
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="H50" t="s">
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -2175,11 +2384,15 @@
       <c r="F51" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H51" s="1" t="s">
+      <c r="G51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>91</v>
       </c>
@@ -2195,11 +2408,14 @@
       <c r="F52" t="s">
         <v>103</v>
       </c>
-      <c r="H52" t="s">
+      <c r="G52" t="s">
+        <v>103</v>
+      </c>
+      <c r="I52" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>108</v>
       </c>
@@ -2215,11 +2431,14 @@
       <c r="F53" t="s">
         <v>103</v>
       </c>
-      <c r="H53" t="s">
+      <c r="G53" t="s">
+        <v>103</v>
+      </c>
+      <c r="I53" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2235,11 +2454,14 @@
       <c r="F54" t="s">
         <v>171</v>
       </c>
-      <c r="H54" t="s">
+      <c r="G54" t="s">
+        <v>193</v>
+      </c>
+      <c r="I54" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>110</v>
       </c>
@@ -2252,14 +2474,17 @@
       <c r="E55" t="s">
         <v>121</v>
       </c>
-      <c r="F55">
-        <v>3</v>
-      </c>
-      <c r="H55" t="s">
+      <c r="F55" t="s">
+        <v>121</v>
+      </c>
+      <c r="G55" t="s">
+        <v>121</v>
+      </c>
+      <c r="I55" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>111</v>
       </c>
@@ -2272,14 +2497,17 @@
       <c r="E56" t="s">
         <v>122</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="s">
+        <v>122</v>
+      </c>
+      <c r="G56">
         <v>0.01</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2295,11 +2523,14 @@
       <c r="F57" t="s">
         <v>124</v>
       </c>
-      <c r="H57" t="s">
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="I57" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -2315,11 +2546,14 @@
       <c r="F58" t="s">
         <v>172</v>
       </c>
-      <c r="H58" t="s">
+      <c r="G58">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I58" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2335,11 +2569,14 @@
       <c r="F59" t="s">
         <v>173</v>
       </c>
-      <c r="H59" t="s">
+      <c r="G59">
+        <v>1.2</v>
+      </c>
+      <c r="I59" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -2355,48 +2592,66 @@
       <c r="F60">
         <v>0</v>
       </c>
-      <c r="H60" t="s">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>174</v>
       </c>
       <c r="F61" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="G61" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>175</v>
       </c>
       <c r="F62" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>176</v>
       </c>
       <c r="F63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="G63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>177</v>
       </c>
       <c r="F64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>178</v>
       </c>
       <c r="F65" t="s">
         <v>180</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Voxel spacing prediction - resnet34, no cos lr
</commit_message>
<xml_diff>
--- a/hyperparameters.xlsx
+++ b/hyperparameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\flagellar\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE87AB50-5C70-49FC-8C3E-BFDFF07FEC19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CEDD2B-9C7E-451E-A8C7-E050FC36DADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9D5827AF-A3F6-4431-B7DE-3210B6AEA3AF}"/>
   </bookViews>
@@ -663,11 +663,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,8 +1009,8 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G60" sqref="G60"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,7 +1182,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6">
@@ -2600,7 +2601,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="3" t="s">
         <v>174</v>
       </c>
       <c r="F61" t="s">
@@ -2622,7 +2623,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="3" t="s">
         <v>176</v>
       </c>
       <c r="F63" t="s">
@@ -2633,7 +2634,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="3" t="s">
         <v>177</v>
       </c>
       <c r="F64" t="s">
@@ -2644,7 +2645,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="4" t="s">
         <v>178</v>
       </c>
       <c r="F65" t="s">

</xml_diff>